<commit_message>
Le tableau était pas bon, là c'est pour de vrai, c'est la fin.
</commit_message>
<xml_diff>
--- a/public/competence/8-1 - BTS SIO - 2025 - Annexe 8-1 - Epreuve E5 - Tableau de synthese.xlsx
+++ b/public/competence/8-1 - BTS SIO - 2025 - Annexe 8-1 - Epreuve E5 - Tableau de synthese.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxim\Desktop\portoflio\public\competence\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8E9181-B8CD-4B18-8D5E-2752540AEA7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834460CE-99B8-4A84-91A1-984E7742F984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -113,18 +113,9 @@
     <t>Veille Technologique sur les moteurs de jeux vidéo</t>
   </si>
   <si>
-    <t>Développement du portfolio en Next.js</t>
-  </si>
-  <si>
     <t>Autoformation sur Unity dans le cadre du projet professionnel</t>
   </si>
   <si>
-    <t>Profil Linkedin</t>
-  </si>
-  <si>
-    <t>Profil GitHub</t>
-  </si>
-  <si>
     <t>Marieteam Java</t>
   </si>
   <si>
@@ -177,6 +168,15 @@
   </si>
   <si>
     <t>01/02/2025 au 30/04/2025</t>
+  </si>
+  <si>
+    <t>Profil Linkedin : https://www.linkedin.com/in/maxime-brunin-860094216/</t>
+  </si>
+  <si>
+    <t>Profil GitHub : https://github.com/MaxBrn</t>
+  </si>
+  <si>
+    <t>Développment du portfolio en Next.js</t>
   </si>
 </sst>
 </file>
@@ -740,6 +740,33 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -755,9 +782,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -780,30 +804,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1116,8 +1116,8 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1130,56 +1130,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="32"/>
+      <c r="H1" s="27"/>
     </row>
     <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="47" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" s="42"/>
-      <c r="H3" s="48"/>
+      <c r="A3" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="29"/>
+      <c r="H3" s="35"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="46"/>
+      <c r="A4" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="33"/>
       <c r="F4" s="12" t="s">
         <v>8</v>
       </c>
@@ -1187,26 +1187,26 @@
         <v>15</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="40"/>
+      <c r="A5" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="48"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="44" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1229,8 +1229,8 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="324.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
-      <c r="B7" s="37"/>
+      <c r="A7" s="40"/>
+      <c r="B7" s="45"/>
       <c r="C7" s="8" t="s">
         <v>9</v>
       </c>
@@ -1286,16 +1286,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="35"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="43"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1334,10 +1334,10 @@
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C9" s="17"/>
       <c r="D9" s="14"/>
@@ -1383,10 +1383,10 @@
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="14"/>
@@ -1432,10 +1432,10 @@
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
@@ -1484,7 +1484,7 @@
         <v>22</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
@@ -1530,10 +1530,10 @@
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
@@ -1579,10 +1579,10 @@
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
@@ -1628,10 +1628,10 @@
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -1677,10 +1677,10 @@
     </row>
     <row r="16" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
@@ -1725,16 +1725,16 @@
       <c r="AQ16"/>
     </row>
     <row r="17" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="29"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="38"/>
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
@@ -1773,10 +1773,10 @@
     </row>
     <row r="18" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
@@ -1821,16 +1821,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="29"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="38"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1869,10 +1869,10 @@
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C20" s="24"/>
       <c r="D20" s="24"/>
@@ -2765,11 +2765,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A19:H19"/>
     <mergeCell ref="A17:H17"/>
     <mergeCell ref="A6:A7"/>
@@ -2777,6 +2772,11 @@
     <mergeCell ref="A8:H8"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
Bon ben allez bonne chance hein
</commit_message>
<xml_diff>
--- a/public/competence/8-1 - BTS SIO - 2025 - Annexe 8-1 - Epreuve E5 - Tableau de synthese.xlsx
+++ b/public/competence/8-1 - BTS SIO - 2025 - Annexe 8-1 - Epreuve E5 - Tableau de synthese.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxim\Desktop\portoflio\public\competence\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834460CE-99B8-4A84-91A1-984E7742F984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E21F7C6-42E6-4E5C-9DAC-615E2A27CEDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -149,9 +149,6 @@
     <t>17/03/2024 au 30/04/2025</t>
   </si>
   <si>
-    <t>Installer un serveur GLPI, gérer les habilitation, mettre en place un collecteur et garantir sa continuité (Marieteam)</t>
-  </si>
-  <si>
     <t>NOM et prénom : Brunin Maxime</t>
   </si>
   <si>
@@ -176,7 +173,10 @@
     <t>Profil GitHub : https://github.com/MaxBrn</t>
   </si>
   <si>
-    <t>Développment du portfolio en Next.js</t>
+    <t>Installer un serveur GLPI, gérer les habilitations, mettre en place un collecteur et garantir sa continuité (Marieteam)</t>
+  </si>
+  <si>
+    <t>Développement du portfolio en Next.js</t>
   </si>
 </sst>
 </file>
@@ -740,9 +740,48 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -765,45 +804,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1116,7 +1116,7 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -1130,56 +1130,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="27"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="29"/>
-      <c r="H3" s="35"/>
+      <c r="A3" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="42"/>
+      <c r="H3" s="48"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="33"/>
+      <c r="A4" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="46"/>
       <c r="F4" s="12" t="s">
         <v>8</v>
       </c>
@@ -1187,26 +1187,26 @@
         <v>15</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="48"/>
+      <c r="A5" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="40"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="36" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1229,8 +1229,8 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="324.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="40"/>
-      <c r="B7" s="45"/>
+      <c r="A7" s="31"/>
+      <c r="B7" s="37"/>
       <c r="C7" s="8" t="s">
         <v>9</v>
       </c>
@@ -1286,16 +1286,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="42"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="43"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="35"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1432,7 +1432,7 @@
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>32</v>
@@ -1582,7 +1582,7 @@
         <v>23</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
@@ -1628,7 +1628,7 @@
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>34</v>
@@ -1677,7 +1677,7 @@
     </row>
     <row r="16" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>34</v>
@@ -1725,16 +1725,16 @@
       <c r="AQ16"/>
     </row>
     <row r="17" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="38"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="29"/>
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
@@ -1821,16 +1821,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="38"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="29"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -2765,6 +2765,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A19:H19"/>
     <mergeCell ref="A17:H17"/>
     <mergeCell ref="A6:A7"/>
@@ -2772,11 +2777,6 @@
     <mergeCell ref="A8:H8"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>